<commit_message>
Atualizei dados e imagens do projeto
</commit_message>
<xml_diff>
--- a/data/vendas_2024.xlsx
+++ b/data/vendas_2024.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lengola_Simão\Jupyter_notebook\Analise_de_dados\Proj_github\Analise_de_dado_2024\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -445,11 +450,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -513,13 +518,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Escritório">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -557,9 +570,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -591,9 +604,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -625,9 +639,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Escritório">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -800,14 +815,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -839,7 +859,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1001</v>
       </c>
@@ -871,7 +891,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1002</v>
       </c>
@@ -903,7 +923,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1003</v>
       </c>
@@ -935,7 +955,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1004</v>
       </c>
@@ -967,7 +987,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1005</v>
       </c>
@@ -999,7 +1019,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1006</v>
       </c>
@@ -1031,7 +1051,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1007</v>
       </c>
@@ -1063,7 +1083,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1008</v>
       </c>
@@ -1095,7 +1115,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1009</v>
       </c>
@@ -1127,7 +1147,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1010</v>
       </c>
@@ -1159,7 +1179,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1011</v>
       </c>
@@ -1191,7 +1211,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1012</v>
       </c>
@@ -1223,7 +1243,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1013</v>
       </c>
@@ -1255,7 +1275,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1014</v>
       </c>
@@ -1287,7 +1307,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1015</v>
       </c>
@@ -1319,7 +1339,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1016</v>
       </c>
@@ -1351,7 +1371,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1017</v>
       </c>
@@ -1383,7 +1403,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1018</v>
       </c>
@@ -1415,7 +1435,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1019</v>
       </c>
@@ -1447,7 +1467,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1020</v>
       </c>
@@ -1479,7 +1499,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1021</v>
       </c>
@@ -1511,7 +1531,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1022</v>
       </c>
@@ -1543,7 +1563,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1023</v>
       </c>
@@ -1575,7 +1595,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1024</v>
       </c>
@@ -1607,7 +1627,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1025</v>
       </c>
@@ -1639,7 +1659,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1026</v>
       </c>
@@ -1671,7 +1691,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1027</v>
       </c>
@@ -1703,7 +1723,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1028</v>
       </c>
@@ -1735,7 +1755,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>1029</v>
       </c>
@@ -1767,7 +1787,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1030</v>
       </c>
@@ -1799,7 +1819,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>1031</v>
       </c>
@@ -1831,7 +1851,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>1032</v>
       </c>
@@ -1863,7 +1883,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>1033</v>
       </c>
@@ -1895,7 +1915,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>1034</v>
       </c>
@@ -1927,7 +1947,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>1035</v>
       </c>
@@ -1959,7 +1979,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>1036</v>
       </c>
@@ -1991,7 +2011,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>1037</v>
       </c>
@@ -2023,7 +2043,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>1038</v>
       </c>
@@ -2055,7 +2075,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>1039</v>
       </c>
@@ -2087,7 +2107,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>1040</v>
       </c>
@@ -2119,7 +2139,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>1041</v>
       </c>
@@ -2151,7 +2171,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>1042</v>
       </c>
@@ -2183,7 +2203,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>1043</v>
       </c>
@@ -2215,7 +2235,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>1044</v>
       </c>
@@ -2247,7 +2267,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>1045</v>
       </c>
@@ -2279,7 +2299,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>1046</v>
       </c>
@@ -2311,7 +2331,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>1047</v>
       </c>
@@ -2343,7 +2363,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>1048</v>
       </c>
@@ -2375,7 +2395,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>1049</v>
       </c>
@@ -2407,7 +2427,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>1050</v>
       </c>
@@ -2439,7 +2459,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>1051</v>
       </c>
@@ -2471,7 +2491,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>1052</v>
       </c>
@@ -2503,7 +2523,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="54" spans="1:10">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>1053</v>
       </c>
@@ -2535,7 +2555,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>1054</v>
       </c>
@@ -2567,7 +2587,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="56" spans="1:10">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>1055</v>
       </c>
@@ -2599,7 +2619,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="57" spans="1:10">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>1056</v>
       </c>
@@ -2631,7 +2651,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="58" spans="1:10">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>1057</v>
       </c>
@@ -2663,7 +2683,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="59" spans="1:10">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>1058</v>
       </c>
@@ -2695,7 +2715,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="60" spans="1:10">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>1059</v>
       </c>
@@ -2727,7 +2747,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="61" spans="1:10">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>1060</v>
       </c>
@@ -2759,7 +2779,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="62" spans="1:10">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>1061</v>
       </c>
@@ -2791,7 +2811,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="63" spans="1:10">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>1062</v>
       </c>
@@ -2823,7 +2843,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="64" spans="1:10">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>1063</v>
       </c>
@@ -2855,7 +2875,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="65" spans="1:10">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>1064</v>
       </c>
@@ -2887,7 +2907,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="66" spans="1:10">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>1065</v>
       </c>
@@ -2919,7 +2939,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="67" spans="1:10">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>1066</v>
       </c>
@@ -2951,7 +2971,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="68" spans="1:10">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>1067</v>
       </c>
@@ -2983,7 +3003,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="69" spans="1:10">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>1068</v>
       </c>
@@ -3015,7 +3035,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="70" spans="1:10">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>1069</v>
       </c>
@@ -3047,7 +3067,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="71" spans="1:10">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>1070</v>
       </c>
@@ -3079,7 +3099,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="72" spans="1:10">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>1071</v>
       </c>
@@ -3111,7 +3131,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="73" spans="1:10">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>1072</v>
       </c>
@@ -3143,7 +3163,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="74" spans="1:10">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>1073</v>
       </c>
@@ -3175,7 +3195,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="75" spans="1:10">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>1074</v>
       </c>
@@ -3207,7 +3227,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="76" spans="1:10">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>1075</v>
       </c>
@@ -3239,7 +3259,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="77" spans="1:10">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>1076</v>
       </c>
@@ -3271,7 +3291,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="78" spans="1:10">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>1077</v>
       </c>
@@ -3303,7 +3323,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="79" spans="1:10">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>1078</v>
       </c>
@@ -3335,7 +3355,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="80" spans="1:10">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>1079</v>
       </c>
@@ -3367,7 +3387,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="81" spans="1:10">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>1080</v>
       </c>
@@ -3399,7 +3419,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="82" spans="1:10">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>1081</v>
       </c>
@@ -3431,7 +3451,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="83" spans="1:10">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>1082</v>
       </c>
@@ -3463,7 +3483,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="84" spans="1:10">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>1083</v>
       </c>
@@ -3495,7 +3515,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="85" spans="1:10">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>1084</v>
       </c>
@@ -3527,7 +3547,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="86" spans="1:10">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>1085</v>
       </c>
@@ -3559,7 +3579,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="87" spans="1:10">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>1086</v>
       </c>
@@ -3591,7 +3611,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="88" spans="1:10">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>1087</v>
       </c>
@@ -3623,7 +3643,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="89" spans="1:10">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>1088</v>
       </c>
@@ -3655,7 +3675,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="90" spans="1:10">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>1089</v>
       </c>
@@ -3687,7 +3707,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="91" spans="1:10">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>1090</v>
       </c>
@@ -3719,7 +3739,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="92" spans="1:10">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>1091</v>
       </c>
@@ -3751,7 +3771,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="93" spans="1:10">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>1092</v>
       </c>
@@ -3783,7 +3803,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="94" spans="1:10">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>1093</v>
       </c>
@@ -3815,7 +3835,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="95" spans="1:10">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>1094</v>
       </c>
@@ -3847,7 +3867,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="96" spans="1:10">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>1095</v>
       </c>
@@ -3879,7 +3899,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="97" spans="1:10">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>1096</v>
       </c>
@@ -3911,7 +3931,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="98" spans="1:10">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>1097</v>
       </c>
@@ -3943,7 +3963,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="99" spans="1:10">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>1098</v>
       </c>
@@ -3975,7 +3995,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="100" spans="1:10">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>1099</v>
       </c>
@@ -4007,7 +4027,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="101" spans="1:10">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>1100</v>
       </c>

</xml_diff>